<commit_message>
Created GUI and finished json
</commit_message>
<xml_diff>
--- a/surveys/Characterization 011020-950.xlsx
+++ b/surveys/Characterization 011020-950.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12435" windowWidth="28800" xWindow="0" yWindow="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Survey Sheet (2)" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="2360-190602" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Map" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Survey Sheet (2)" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2360-190602" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Map" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName localSheetId="1" name="_2360">#REF!</definedName>
-    <definedName localSheetId="2" name="_2360">#REF!</definedName>
-    <definedName localSheetId="0" name="_2360">#REF!</definedName>
+    <definedName name="_2360" localSheetId="1">#REF!</definedName>
+    <definedName name="_2360" localSheetId="2">#REF!</definedName>
+    <definedName name="_2360" localSheetId="0">#REF!</definedName>
     <definedName name="_2360">#REF!</definedName>
-    <definedName localSheetId="0" name="_xlnm.Print_Area">'Survey Sheet (2)'!$A$1:$Y$41</definedName>
-    <definedName localSheetId="1" name="_xlnm.Print_Titles">'2360-190602'!$1:$17</definedName>
-    <definedName localSheetId="1" name="_xlnm.Print_Area">'2360-190602'!$A$1:$S$39</definedName>
-    <definedName localSheetId="2" name="_xlnm.Print_Area">'Map'!$A$1:$BY$45</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Survey Sheet (2)'!$A$1:$Y$41</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">'2360-190602'!$1:$17</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'2360-190602'!$A$1:$S$39</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Map'!$A$1:$BY$45</definedName>
   </definedNames>
   <calcPr calcId="152511" fullCalcOnLoad="1"/>
 </workbook>
@@ -27,10 +27,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt formatCode=";;;" numFmtId="164"/>
-    <numFmt formatCode="m/d/yy;@" numFmtId="165"/>
-    <numFmt formatCode="0.0" numFmtId="166"/>
-    <numFmt formatCode="m/d/yyyy;@" numFmtId="167"/>
+    <numFmt numFmtId="164" formatCode=";;;"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -1966,1882 +1966,1882 @@
     </border>
   </borders>
   <cellStyleXfs count="4">
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="606">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="24" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="50" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="47" fillId="0" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="47" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="50" fillId="0" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="47" fillId="0" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="47" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="56" fillId="4" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="56" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="62" fillId="4" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="62" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="59" fillId="4" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="59" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="63" fillId="4" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="63" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="64" fillId="4" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="64" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="60" fillId="4" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="60" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="61" fillId="4" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="61" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="3" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="8" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="9" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="18" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="19" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="18" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="24" fillId="3" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="25" fillId="3" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="25" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="26" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="30" fillId="3" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="30" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="25" fillId="3" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="26" fillId="3" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="26" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="29" fillId="3" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="31" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="31" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="5" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="18" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="32" fillId="3" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="33" fillId="3" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="33" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="33" fillId="3" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="33" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="34" fillId="3" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="34" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="36" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="36" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="34" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="37" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="34" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="37" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="35" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="35" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="38" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="38" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="39" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="39" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="33" fillId="3" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="33" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="40" fillId="3" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="40" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="8" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="8" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="41" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="41" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="15" fillId="3" fontId="11" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="42" fillId="3" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="42" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="47" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="8" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="41" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="41" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="25" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="25" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="15" fillId="3" fontId="11" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="12" fillId="3" fontId="11" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="13" fillId="3" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="13" fillId="3" fontId="11" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="14" fillId="3" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="51" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="51" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="52" fillId="5" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="51" fillId="5" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="18" fillId="3" fontId="11" numFmtId="0" pivotButton="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="52" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="51" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="15" fillId="3" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="15" fillId="3" fontId="11" numFmtId="0" pivotButton="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="14" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="52" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="52" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="15" fillId="3" fontId="15" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="41" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="41" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="10" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="45" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="45" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="15" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="50" fillId="0" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="67" fillId="0" fontId="3" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="67" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="68" fillId="0" fontId="3" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="68" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="69" fillId="0" fontId="3" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="69" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="66" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="66" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="70" fillId="0" fontId="3" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="70" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="18" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="73" fillId="0" fontId="3" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="73" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="79" fillId="0" fontId="3" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="79" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="80" fillId="0" fontId="3" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="80" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="14" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="10" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="1" fontId="10" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="10" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="1" fontId="10" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" applyProtection="1" borderId="10" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="44" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="44" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="45" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="45" fillId="2" fontId="3" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="45" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="45" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="51" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="51" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="65" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="51" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="65" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="51" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="52" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="52" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="66" fillId="2" fontId="17" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="66" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="71" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="10" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="71" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="72" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="72" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="42" fillId="2" fontId="3" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="42" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="75" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="48" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="75" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="77" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="77" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="55" fillId="2" fontId="3" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="55" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="78" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="78" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="43" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="10" fillId="2" fontId="3" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="43" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="10" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="10" fillId="2" fontId="3" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="29" fillId="3" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="10" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="24" fillId="0" fontId="22" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="25" fillId="0" fontId="22" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="31" fillId="0" fontId="22" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="31" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="47" fillId="0" fontId="22" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="47" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="22" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="22" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="81" fillId="0" fontId="22" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="81" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="47" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="81" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="19" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="47" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="81" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="19" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="19" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="0" fillId="0" fontId="23" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="47" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="0" fillId="0" fontId="23" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="0" fillId="0" fontId="23" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="20" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="1" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="1" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="1" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="23" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="25" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="25" fillId="0" fontId="19" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="47" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="14" fontId="23" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="25" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="31" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="81" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="24" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="81" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="24" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="24" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="23" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="80" fillId="3" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="87" fillId="3" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="78" fillId="6" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="76" fillId="3" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="79" fillId="0" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="88" fillId="0" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="87" fillId="0" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="88" fillId="6" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="87" fillId="6" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="55" fillId="6" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="80" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="87" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="6" borderId="78" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="76" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="79" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="88" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="87" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="6" borderId="88" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="6" borderId="87" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="6" borderId="55" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="77" fillId="6" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="6" borderId="77" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="75" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="73" fillId="3" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="89" fillId="3" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="72" fillId="6" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="74" fillId="3" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="67" fillId="0" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="19" fillId="0" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="89" fillId="0" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="19" fillId="6" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="89" fillId="6" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="42" fillId="6" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="75" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="73" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="89" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="6" borderId="72" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="74" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="67" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="89" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="6" borderId="19" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="6" borderId="89" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="6" borderId="42" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="45" fillId="6" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="6" borderId="45" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="65" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="71" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="19" fillId="3" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="70" fillId="3" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="90" fillId="3" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="91" fillId="6" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="84" fillId="3" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="69" fillId="0" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="3" fillId="0" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="90" fillId="0" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="92" fillId="6" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="93" fillId="6" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="94" fillId="0" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="94" fillId="6" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="7" fillId="6" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="65" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="71" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="70" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="90" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="6" borderId="91" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="84" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="69" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="90" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="6" borderId="92" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="6" borderId="93" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="94" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="6" borderId="94" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="6" borderId="7" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="95" fillId="6" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="6" borderId="95" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="96" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="64" fillId="0" fontId="27" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="96" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="64" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="97" fillId="0" fontId="27" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="97" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="60" fillId="0" fontId="27" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="60" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="58" fillId="0" fontId="27" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="58" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="30" fillId="0" fontId="27" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="30" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="62" fillId="0" fontId="27" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="62" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="59" fillId="0" fontId="27" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="59" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="61" fillId="0" fontId="27" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="61" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="56" fillId="0" fontId="28" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="56" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="21" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="103" fillId="0" fontId="25" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="24" fillId="0" fontId="30" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="103" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="81" fillId="0" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="14" fillId="0" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="77" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="105" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="106" fillId="0" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="82" fillId="0" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="45" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="107" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="45" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="107" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="45" fillId="6" fontId="4" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="107" fillId="6" fontId="4" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="95" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="108" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="81" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="77" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="105" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="106" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="82" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="45" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="107" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="107" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="6" borderId="45" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="6" borderId="107" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="95" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="108" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="23" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="64" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="59" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="64" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="59" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="6" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="5" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="2" fillId="6" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="2" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="6" fillId="6" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="6" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="5" fillId="6" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="5" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="18" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="15" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="11" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="18" fillId="6" fontId="4" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="14" fontId="4" fillId="6" borderId="18" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="15" fillId="6" fontId="4" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="6" borderId="15" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="11" fillId="6" fontId="4" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="6" borderId="11" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="18" fillId="6" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="18" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="15" fillId="6" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="15" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="11" fillId="6" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="11" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="7" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="4" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="6" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="5" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="47" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="47" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="20" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="10" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="15" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="15" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="11" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="48" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="48" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="54" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="54" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="49" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="49" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="53" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="53" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="54" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="49" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="49" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="53" fillId="6" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="53" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="54" fillId="6" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="54" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="49" fillId="6" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="49" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="20" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="23" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="112" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="58" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="59" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="104" fillId="0" fontId="25" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="111" fillId="0" fontId="25" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="32" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="33" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="39" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="33" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="110" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="8" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="112" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="58" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="59" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="104" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="111" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="33" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="39" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="33" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="110" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="41" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="41" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="82" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="82" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="103" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="109" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="109" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="100" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="100" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="99" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="103" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="109" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="109" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="100" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="100" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="99" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="102" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="102" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="99" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="98" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="42" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="99" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="98" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="42" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="6" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="7" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="51" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="41" fillId="6" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="10" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="15" fillId="6" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="4" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="6" fillId="6" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="7" fillId="6" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="4" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="6" fillId="6" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="5" fillId="6" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="15" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="42" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="10" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="15" fillId="6" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="51" fillId="6" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="41" fillId="6" fontId="20" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="82" fillId="6" fontId="20" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="15" fillId="6" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="11" fillId="6" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="10" fillId="6" fontId="4" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="15" fillId="6" fontId="20" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="3">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="10" fillId="6" fontId="4" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="15" fillId="6" fontId="20" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="3">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="15" fillId="6" fontId="20" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="42" fillId="6" fontId="20" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="15" fillId="6" fontId="20" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="11" fillId="6" fontId="20" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="10" fillId="6" fontId="4" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="15" fillId="6" fontId="20" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="3">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="10" fillId="6" fontId="4" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="3">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="15" fillId="6" fontId="4" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="3">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="15" fillId="6" fontId="20" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="42" fillId="6" fontId="20" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="10" fillId="6" fontId="4" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="15" fillId="6" fontId="4" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="11" fillId="6" fontId="4" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="10" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="15" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="42" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="15" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="42" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="11" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="18" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="10" fillId="6" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="15" fillId="6" fontId="20" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="42" fillId="6" fontId="20" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="15" fillId="6" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="42" fillId="6" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="15" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="11" fillId="6" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="54" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="55" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="48" fillId="0" fontId="29" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="54" fillId="0" fontId="29" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="55" fillId="0" fontId="29" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="48" fillId="0" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="54" fillId="0" fontId="20" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="55" fillId="0" fontId="20" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="49" fillId="0" fontId="20" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="53" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="13" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="14" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="27" fillId="0" fontId="25" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="29" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="27" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="28" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="29" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="25" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="31" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="58" fillId="0" fontId="29" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="51" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="41" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="6" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="7" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="42" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="15" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="51" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="6" borderId="41" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="6" borderId="82" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="6" borderId="10" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="6" borderId="15" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="6" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="6" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="6" borderId="15" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="6" borderId="42" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="6" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="6" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="6" borderId="10" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="20" fillId="6" borderId="15" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="6" borderId="10" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="6" borderId="15" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="20" fillId="6" borderId="15" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="20" fillId="6" borderId="42" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="6" borderId="10" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="6" borderId="15" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="6" borderId="11" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="42" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="42" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="6" borderId="10" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="6" borderId="15" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="6" borderId="42" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="15" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="42" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="15" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="11" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="54" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="55" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="29" fillId="0" borderId="48" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="29" fillId="0" borderId="54" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="29" fillId="0" borderId="55" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="48" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="54" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="55" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="49" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="53" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="28" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="31" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="58" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="64" fillId="0" fontId="29" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="64" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="99" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="100" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="99" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="102" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="85" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="101" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="99" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="100" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="99" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="102" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="85" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="101" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="86" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="86" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="99" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="98" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="57" fillId="0" fontId="28" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="99" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="98" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="57" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="58" fillId="0" fontId="28" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="58" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="59" fillId="0" fontId="28" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="59" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="84" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="84" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="6" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="7" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="74" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="74" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="15" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="15" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="42" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="42" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="76" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="76" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="54" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="54" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="55" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="55" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="74" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="74" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="15" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="42" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="42" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="19" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="76" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="76" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="54" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="54" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="55" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="55" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="26" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="19" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="10" fillId="0" fontId="3" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="42" fillId="0" fontId="3" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="84" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="42" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="84" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="6" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="7" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="48" fillId="0" fontId="3" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="55" fillId="0" fontId="3" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="49" fillId="0" fontId="3" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="10" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="42" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="11" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="57" fillId="4" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="48" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="55" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="49" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="42" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="57" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="58" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="59" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="10" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="42" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="11" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="11" fillId="0" fontId="3" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="53" fillId="3" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="53" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="54" fillId="3" fontId="16" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="54" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="55" fillId="3" fontId="16" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="55" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="10" fillId="0" fontId="3" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="42" fillId="0" fontId="3" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="51" fillId="0" fontId="3" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="82" fillId="0" fontId="3" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="10" fillId="3" fontId="3" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="42" fillId="3" fontId="3" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="11" fillId="3" fontId="3" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="10" fillId="2" fontId="3" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="42" fillId="2" fontId="3" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="11" fillId="2" fontId="3" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="10" fillId="0" fontId="3" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="42" fillId="0" fontId="3" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="10" fillId="0" fontId="3" numFmtId="167" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="42" fillId="0" fontId="3" numFmtId="167" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="10" fillId="3" fontId="3" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="42" fillId="3" fontId="3" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="11" fillId="3" fontId="3" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="43" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="46" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="83" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="85" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="86" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="43" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="46" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="42" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="51" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="82" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="3" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="3" borderId="42" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="3" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="10" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="42" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="11" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="42" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="42" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="42" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="46" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="83" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="85" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="86" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="4" fillId="2" fontId="3" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="4" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="5" fillId="2" fontId="3" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="5" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="6" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="7" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="4" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="6" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="5" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="10" fillId="2" fontId="3" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="10" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="11" fillId="2" fontId="3" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="11" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="12" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="13" fillId="0" fontId="21" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="14" fillId="0" fontId="21" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="20" fillId="0" fontId="21" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="21" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="21" fillId="0" fontId="21" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="16" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="13" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="17" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="22" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="1" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="23" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="10" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="11" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="18" fillId="3" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="15" fillId="3" fontId="16" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="42" fillId="3" fontId="16" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="42" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="28" fillId="3" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="29" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="27" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="48" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="28" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="49" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="49" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="10" fillId="2" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="10" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="15" fillId="2" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="15" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="11" fillId="2" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="11" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="4" fillId="2" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="6" fillId="2" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="6" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="5" fillId="2" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="5" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="10" fillId="2" fontId="4" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="10" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="15" fillId="2" fontId="4" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="15" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="11" fillId="2" fontId="4" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="11" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="55" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="55" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="48" fillId="2" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="48" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="54" fillId="2" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="54" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="49" fillId="2" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="49" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="131" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="131" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" applyProtection="1" borderId="131" fillId="6" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="131" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="127" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="127" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf borderId="15" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="11" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" applyProtection="1" borderId="127" fillId="6" fontId="4" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="14" fontId="4" fillId="6" borderId="127" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="127" fillId="6" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="127" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="108" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="108" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" applyProtection="1" borderId="122" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="122" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="121" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="121" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="17" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="20" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="51" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="41" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="106" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="129" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="106" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="129" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf borderId="54" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="49" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" applyProtection="1" borderId="129" fillId="6" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="129" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="130" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="23" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="123" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="124" fillId="0" fontId="25" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="111" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="33" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="125" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="110" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="126" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="130" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="123" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="124" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="111" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="125" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="110" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="126" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf borderId="82" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="99" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="102" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="115" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="98" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="107" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="82" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="99" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="102" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="115" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="98" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="107" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf borderId="42" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="122" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="52" fillId="6" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="121" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="45" fillId="6" fontId="4" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="121" fillId="6" fontId="4" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="45" fillId="6" fontId="4" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="121" fillId="6" fontId="4" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="121" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="107" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="45" fillId="6" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="11" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf borderId="55" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="77" fillId="0" fontId="29" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="77" fillId="0" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="118" fillId="0" fontId="4" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="105" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="119" fillId="0" fontId="25" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="27" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="29" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="120" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="64" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="109" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="114" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="113" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="86" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="117" fillId="0" fontId="28" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="122" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="52" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="121" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="6" borderId="45" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="6" borderId="121" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="6" borderId="45" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="6" borderId="121" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="121" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="107" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="6" borderId="45" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="166" fontId="29" fillId="0" borderId="77" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="77" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="118" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="105" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="119" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="120" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="109" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="114" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="113" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="117" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="69" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="69" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="67" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="67" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="79" fillId="6" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="79" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="122" fillId="2" fontId="3" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="122" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="108" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="108" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="122" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="122" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="121" fillId="2" fontId="3" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="121" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="105" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="105" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="14" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" applyProtection="1" borderId="118" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="118" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="121" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="121" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf borderId="21" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="22" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="132" fillId="3" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="44" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="46" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="114" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="44" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="133" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="83" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" applyProtection="1" borderId="118" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="132" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="114" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="44" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="133" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="118" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="45" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="45" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="121" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="45" fillId="0" fontId="3" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="45" fillId="0" fontId="3" numFmtId="167" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="45" fillId="3" fontId="3" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="121" fillId="3" fontId="3" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="45" fillId="0" fontId="3" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="52" fillId="0" fontId="3" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="45" fillId="3" fontId="3" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="121" fillId="3" fontId="3" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="45" fillId="2" fontId="3" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="121" fillId="2" fontId="3" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="121" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="107" fillId="3" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="121" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="45" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="45" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="45" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="121" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="45" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="52" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="3" borderId="45" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="3" borderId="121" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="45" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="121" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="121" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="107" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="45" fillId="0" fontId="3" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="121" fillId="0" fontId="3" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="105" fillId="3" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="45" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="121" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="105" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="77" fillId="0" fontId="3" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="118" fillId="0" fontId="3" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="117" fillId="4" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="77" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="118" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="117" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="69" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="69" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="67" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="67" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="79" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="79" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="122" fillId="2" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="122" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="121" fillId="2" fontId="4" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="121" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="121" fillId="2" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="121" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="105" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="105" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="118" fillId="2" fontId="4" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="118" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="0"/>
+      <protection locked="0" hidden="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Normal 4" xfId="2"/>
     <cellStyle name="Normal 4 2" xfId="3"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -4182,23 +4182,23 @@
   </sheetPr>
   <dimension ref="A1:AJ41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0" zoomScaleNormal="100">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J5" sqref="J5:Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" max="25" min="1" style="213" width="7.28515625"/>
-    <col customWidth="1" max="27" min="26" style="213" width="9.140625"/>
-    <col bestFit="1" customWidth="1" max="28" min="28" style="213" width="11.42578125"/>
-    <col customWidth="1" max="29" min="29" style="213" width="9.140625"/>
-    <col bestFit="1" customWidth="1" max="30" min="30" style="213" width="10"/>
-    <col customWidth="1" max="34" min="31" style="213" width="9.140625"/>
-    <col bestFit="1" customWidth="1" max="35" min="35" style="213" width="10.85546875"/>
-    <col customWidth="1" max="16384" min="36" style="213" width="9.140625"/>
+    <col width="7.28515625" customWidth="1" style="213" min="1" max="25"/>
+    <col width="9.140625" customWidth="1" style="213" min="26" max="27"/>
+    <col width="11.42578125" bestFit="1" customWidth="1" style="213" min="28" max="28"/>
+    <col width="9.140625" customWidth="1" style="213" min="29" max="29"/>
+    <col width="10" bestFit="1" customWidth="1" style="213" min="30" max="30"/>
+    <col width="9.140625" customWidth="1" style="213" min="31" max="34"/>
+    <col width="10.85546875" bestFit="1" customWidth="1" style="213" min="35" max="35"/>
+    <col width="9.140625" customWidth="1" style="213" min="36" max="16384"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="18" r="1" s="91" thickTop="1">
+    <row r="1" ht="18" customHeight="1" s="91" thickTop="1">
       <c r="A1" s="490" t="inlineStr">
         <is>
           <t>Survey Number</t>
@@ -4234,7 +4234,7 @@
       <c r="Y1" s="213" t="n"/>
       <c r="Z1" s="213" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="2" s="91">
+    <row r="2" ht="18" customHeight="1" s="91">
       <c r="A2" s="494" t="inlineStr">
         <is>
           <t>Date Counted</t>
@@ -4266,7 +4266,7 @@
       <c r="Y2" s="213" t="n"/>
       <c r="Z2" s="213" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="3" s="91" thickBot="1">
+    <row r="3" ht="18" customHeight="1" s="91" thickBot="1">
       <c r="A3" s="494" t="inlineStr">
         <is>
           <t>Survey Tech</t>
@@ -4300,7 +4300,7 @@
       <c r="Y3" s="232" t="n"/>
       <c r="Z3" s="213" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="4" s="91" thickTop="1">
+    <row r="4" ht="18" customHeight="1" s="91" thickTop="1">
       <c r="A4" s="494" t="inlineStr">
         <is>
           <t>Count Room Tech</t>
@@ -4343,7 +4343,7 @@
       <c r="X4" s="491" t="n"/>
       <c r="Y4" s="492" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="5" s="91">
+    <row r="5" ht="18" customHeight="1" s="91">
       <c r="A5" s="494" t="inlineStr">
         <is>
           <t>Date Counted</t>
@@ -4385,7 +4385,7 @@
       <c r="X5" s="503" t="n"/>
       <c r="Y5" s="504" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="6" s="91" thickBot="1">
+    <row r="6" ht="18" customHeight="1" s="91" thickBot="1">
       <c r="A6" s="494" t="inlineStr">
         <is>
           <t>Survey Type</t>
@@ -4420,7 +4420,7 @@
       <c r="X6" s="508" t="n"/>
       <c r="Y6" s="509" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="7" s="91" thickBot="1" thickTop="1">
+    <row r="7" ht="18" customHeight="1" s="91" thickBot="1" thickTop="1">
       <c r="A7" s="510" t="inlineStr">
         <is>
           <t>Level Of Posting</t>
@@ -4459,7 +4459,7 @@
       <c r="X7" s="506" t="n"/>
       <c r="Y7" s="515" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="8" s="91" thickBot="1" thickTop="1">
+    <row r="8" ht="18" customHeight="1" s="91" thickBot="1" thickTop="1">
       <c r="A8" s="516" t="inlineStr">
         <is>
           <t>Building Material Background - cpm</t>
@@ -4510,7 +4510,7 @@
       <c r="X8" s="519" t="n"/>
       <c r="Y8" s="521" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="9" s="91" thickBot="1" thickTop="1">
+    <row r="9" ht="18" customHeight="1" s="91" thickBot="1" thickTop="1">
       <c r="A9" s="522" t="inlineStr">
         <is>
           <t>Brick</t>
@@ -4569,7 +4569,7 @@
       <c r="X9" s="524" t="n"/>
       <c r="Y9" s="527" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="10" s="91" thickTop="1">
+    <row r="10" ht="18" customHeight="1" s="91" thickTop="1">
       <c r="A10" s="528" t="inlineStr">
         <is>
           <t>Concrete</t>
@@ -4620,7 +4620,7 @@
       <c r="X10" s="491" t="n"/>
       <c r="Y10" s="492" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="11" s="91">
+    <row r="11" ht="18" customHeight="1" s="91">
       <c r="A11" s="528" t="inlineStr">
         <is>
           <t>Linoleum</t>
@@ -4673,7 +4673,7 @@
       <c r="X11" s="495" t="n"/>
       <c r="Y11" s="496" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="12" s="91">
+    <row r="12" ht="18" customHeight="1" s="91">
       <c r="A12" s="528" t="inlineStr">
         <is>
           <t>Drywall</t>
@@ -4732,7 +4732,7 @@
       <c r="AI12" s="213" t="n"/>
       <c r="AJ12" s="213" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="13" s="91">
+    <row r="13" ht="18" customHeight="1" s="91">
       <c r="A13" s="528" t="inlineStr">
         <is>
           <t>Metal</t>
@@ -4797,7 +4797,7 @@
       <c r="AI13" s="213" t="n"/>
       <c r="AJ13" s="213" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="14" s="91">
+    <row r="14" ht="18" customHeight="1" s="91">
       <c r="A14" s="528" t="inlineStr">
         <is>
           <t>Ceiling Tile</t>
@@ -4862,7 +4862,7 @@
       <c r="AI14" s="213" t="n"/>
       <c r="AJ14" s="213" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="15" s="91">
+    <row r="15" ht="18" customHeight="1" s="91">
       <c r="A15" s="528" t="inlineStr">
         <is>
           <t>Wood</t>
@@ -4919,7 +4919,7 @@
       <c r="AI15" s="213" t="n"/>
       <c r="AJ15" s="213" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="16" s="91">
+    <row r="16" ht="18" customHeight="1" s="91">
       <c r="A16" s="538" t="n"/>
       <c r="B16" s="495" t="n"/>
       <c r="C16" s="495" t="n"/>
@@ -4968,7 +4968,7 @@
       <c r="AI16" s="213" t="n"/>
       <c r="AJ16" s="213" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="17" s="91">
+    <row r="17" ht="18" customHeight="1" s="91">
       <c r="A17" s="538" t="n"/>
       <c r="B17" s="495" t="n"/>
       <c r="C17" s="495" t="n"/>
@@ -5017,7 +5017,7 @@
       <c r="AI17" s="213" t="n"/>
       <c r="AJ17" s="213" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="18" s="91" thickBot="1">
+    <row r="18" ht="18" customHeight="1" s="91" thickBot="1">
       <c r="A18" s="538" t="n"/>
       <c r="B18" s="495" t="n"/>
       <c r="C18" s="495" t="n"/>
@@ -5076,7 +5076,7 @@
       <c r="AI18" s="213" t="n"/>
       <c r="AJ18" s="213" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="19" s="91" thickBot="1" thickTop="1">
+    <row r="19" ht="18" customHeight="1" s="91" thickBot="1" thickTop="1">
       <c r="A19" s="545" t="n"/>
       <c r="B19" s="511" t="n"/>
       <c r="C19" s="511" t="n"/>
@@ -5125,7 +5125,7 @@
       <c r="AI19" s="213" t="n"/>
       <c r="AJ19" s="213" t="n"/>
     </row>
-    <row customHeight="1" ht="18" r="20" s="91" thickBot="1" thickTop="1">
+    <row r="20" ht="18" customHeight="1" s="91" thickBot="1" thickTop="1">
       <c r="A20" s="212" t="inlineStr">
         <is>
           <t>Note</t>
@@ -5184,7 +5184,7 @@
       <c r="X20" s="524" t="n"/>
       <c r="Y20" s="527" t="n"/>
     </row>
-    <row customHeight="1" ht="49.9" r="21" s="91" thickBot="1" thickTop="1">
+    <row r="21" ht="49.9" customHeight="1" s="91" thickBot="1" thickTop="1">
       <c r="A21" s="209" t="inlineStr">
         <is>
           <t>No</t>
@@ -5291,7 +5291,7 @@
         </is>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="19.9" r="22" s="160" thickTop="1">
+    <row r="22" ht="19.9" customFormat="1" customHeight="1" s="160" thickTop="1">
       <c r="A22" s="200" t="n">
         <v>1</v>
       </c>
@@ -5358,7 +5358,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="19.9" r="23" s="160">
+    <row r="23" ht="19.9" customFormat="1" customHeight="1" s="160">
       <c r="A23" s="185" t="n">
         <v>2</v>
       </c>
@@ -5433,7 +5433,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="19.9" r="24" s="160">
+    <row r="24" ht="19.9" customFormat="1" customHeight="1" s="160">
       <c r="A24" s="184" t="n">
         <v>3</v>
       </c>
@@ -5508,7 +5508,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="19.9" r="25" s="160">
+    <row r="25" ht="19.9" customFormat="1" customHeight="1" s="160">
       <c r="A25" s="184" t="n">
         <v>4</v>
       </c>
@@ -5575,7 +5575,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="19.9" r="26" s="160">
+    <row r="26" ht="19.9" customFormat="1" customHeight="1" s="160">
       <c r="A26" s="184" t="n">
         <v>5</v>
       </c>
@@ -5650,7 +5650,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="19.9" r="27" s="160">
+    <row r="27" ht="19.9" customFormat="1" customHeight="1" s="160">
       <c r="A27" s="184" t="n">
         <v>6</v>
       </c>
@@ -5725,7 +5725,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="19.9" r="28" s="160">
+    <row r="28" ht="19.9" customFormat="1" customHeight="1" s="160">
       <c r="A28" s="184" t="n">
         <v>7</v>
       </c>
@@ -5792,7 +5792,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="19.9" r="29" s="160">
+    <row r="29" ht="19.9" customFormat="1" customHeight="1" s="160">
       <c r="A29" s="184" t="n">
         <v>8</v>
       </c>
@@ -5867,7 +5867,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="19.9" r="30" s="160">
+    <row r="30" ht="19.9" customFormat="1" customHeight="1" s="160">
       <c r="A30" s="184" t="n">
         <v>9</v>
       </c>
@@ -5942,7 +5942,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="19.9" r="31" s="160">
+    <row r="31" ht="19.9" customFormat="1" customHeight="1" s="160">
       <c r="A31" s="184" t="n"/>
       <c r="B31" s="557" t="n"/>
       <c r="C31" s="495" t="n"/>
@@ -5999,7 +5999,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="19.9" r="32" s="160">
+    <row r="32" ht="19.9" customFormat="1" customHeight="1" s="160">
       <c r="A32" s="184" t="n"/>
       <c r="B32" s="557" t="n"/>
       <c r="C32" s="495" t="n"/>
@@ -6056,7 +6056,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="19.9" r="33" s="160">
+    <row r="33" ht="19.9" customFormat="1" customHeight="1" s="160">
       <c r="A33" s="185" t="n"/>
       <c r="B33" s="557" t="n"/>
       <c r="C33" s="495" t="n"/>
@@ -6113,7 +6113,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="19.9" r="34" s="160">
+    <row r="34" ht="19.9" customFormat="1" customHeight="1" s="160">
       <c r="A34" s="185" t="n"/>
       <c r="B34" s="557" t="n"/>
       <c r="C34" s="495" t="n"/>
@@ -6170,7 +6170,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="19.9" r="35" s="160">
+    <row r="35" ht="19.9" customFormat="1" customHeight="1" s="160">
       <c r="A35" s="184" t="n"/>
       <c r="B35" s="557" t="n"/>
       <c r="C35" s="495" t="n"/>
@@ -6227,7 +6227,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="19.9" r="36" s="160">
+    <row r="36" ht="19.9" customFormat="1" customHeight="1" s="160">
       <c r="A36" s="184" t="n"/>
       <c r="B36" s="557" t="n"/>
       <c r="C36" s="495" t="n"/>
@@ -6284,7 +6284,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="19.9" r="37" s="160">
+    <row r="37" ht="19.9" customFormat="1" customHeight="1" s="160">
       <c r="A37" s="185" t="n"/>
       <c r="B37" s="557" t="n"/>
       <c r="C37" s="495" t="n"/>
@@ -6341,7 +6341,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="19.9" r="38" s="160">
+    <row r="38" ht="19.9" customFormat="1" customHeight="1" s="160">
       <c r="A38" s="184" t="n"/>
       <c r="B38" s="557" t="n"/>
       <c r="C38" s="495" t="n"/>
@@ -6398,7 +6398,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="19.9" r="39" s="160">
+    <row r="39" ht="19.9" customFormat="1" customHeight="1" s="160">
       <c r="A39" s="184" t="n"/>
       <c r="B39" s="557" t="n"/>
       <c r="C39" s="495" t="n"/>
@@ -6455,7 +6455,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="19.9" r="40" s="160">
+    <row r="40" ht="19.9" customFormat="1" customHeight="1" s="160">
       <c r="A40" s="184" t="n"/>
       <c r="B40" s="557" t="n"/>
       <c r="C40" s="495" t="n"/>
@@ -6512,7 +6512,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="19.9" r="41" s="160" thickBot="1">
+    <row r="41" ht="19.9" customFormat="1" customHeight="1" s="160" thickBot="1">
       <c r="A41" s="172" t="n"/>
       <c r="B41" s="558" t="n"/>
       <c r="C41" s="511" t="n"/>
@@ -6569,7 +6569,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="13.5" r="42" s="91" thickTop="1"/>
+    <row r="42" ht="13.5" customHeight="1" s="91" thickTop="1"/>
   </sheetData>
   <mergeCells count="111">
     <mergeCell ref="B40:G40"/>
@@ -6685,8 +6685,8 @@
     <mergeCell ref="H4:I4"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
-  <pageMargins bottom="0.25" footer="0" header="0" left="0.25" right="0.25" top="0.25"/>
-  <pageSetup horizontalDpi="4294967293" orientation="landscape" scale="73"/>
+  <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>
+  <pageSetup orientation="landscape" scale="73" horizontalDpi="4294967293"/>
 </worksheet>
 </file>
 
@@ -6698,23 +6698,23 @@
   </sheetPr>
   <dimension ref="A1:BC51"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0" zoomScaleNormal="100">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A18" sqref="A18:H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="114" width="3.42578125"/>
-    <col customWidth="1" max="3" min="2" style="114" width="10.42578125"/>
-    <col customWidth="1" max="4" min="4" style="114" width="18.28515625"/>
-    <col customWidth="1" max="5" min="5" style="114" width="5.28515625"/>
-    <col customWidth="1" max="7" min="6" style="114" width="2.5703125"/>
-    <col customWidth="1" max="8" min="8" style="114" width="5.28515625"/>
-    <col customWidth="1" max="19" min="9" style="114" width="7.42578125"/>
-    <col customWidth="1" max="16384" min="20" style="114" width="9.140625"/>
+    <col width="3.42578125" customWidth="1" style="114" min="1" max="1"/>
+    <col width="10.42578125" customWidth="1" style="114" min="2" max="3"/>
+    <col width="18.28515625" customWidth="1" style="114" min="4" max="4"/>
+    <col width="5.28515625" customWidth="1" style="114" min="5" max="5"/>
+    <col width="2.5703125" customWidth="1" style="114" min="6" max="7"/>
+    <col width="5.28515625" customWidth="1" style="114" min="8" max="8"/>
+    <col width="7.42578125" customWidth="1" style="114" min="9" max="19"/>
+    <col width="9.140625" customWidth="1" style="114" min="20" max="16384"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="39" r="1" s="91" thickBot="1">
+    <row r="1" ht="39" customHeight="1" s="91" thickBot="1">
       <c r="A1" s="442" t="n"/>
       <c r="B1" s="506" t="n"/>
       <c r="C1" s="506" t="n"/>
@@ -6735,7 +6735,7 @@
       <c r="R1" s="506" t="n"/>
       <c r="S1" s="506" t="n"/>
     </row>
-    <row customHeight="1" ht="13.5" r="2" s="91" thickTop="1">
+    <row r="2" ht="13.5" customHeight="1" s="91" thickTop="1">
       <c r="A2" s="14" t="n"/>
       <c r="B2" s="15" t="inlineStr">
         <is>
@@ -6772,7 +6772,7 @@
       <c r="R2" s="491" t="n"/>
       <c r="S2" s="492" t="n"/>
     </row>
-    <row customHeight="1" ht="13.5" r="3" s="91">
+    <row r="3" ht="13.5" customHeight="1" s="91">
       <c r="A3" s="16" t="n"/>
       <c r="B3" s="17" t="inlineStr">
         <is>
@@ -6807,7 +6807,7 @@
       <c r="R3" s="503" t="n"/>
       <c r="S3" s="504" t="n"/>
     </row>
-    <row customHeight="1" ht="13.5" r="4" s="91" thickBot="1">
+    <row r="4" ht="13.5" customHeight="1" s="91" thickBot="1">
       <c r="A4" s="18" t="n"/>
       <c r="B4" s="19" t="inlineStr">
         <is>
@@ -6836,7 +6836,7 @@
       <c r="R4" s="506" t="n"/>
       <c r="S4" s="515" t="n"/>
     </row>
-    <row customHeight="1" ht="13.5" r="5" s="91" thickTop="1">
+    <row r="5" ht="13.5" customHeight="1" s="91" thickTop="1">
       <c r="A5" s="20" t="n"/>
       <c r="B5" s="19" t="inlineStr">
         <is>
@@ -6885,7 +6885,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="13.5" r="6" s="91">
+    <row r="6" ht="13.5" customHeight="1" s="91">
       <c r="A6" s="31" t="n"/>
       <c r="B6" s="32" t="inlineStr">
         <is>
@@ -6944,7 +6944,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="13.5" r="7" s="91">
+    <row r="7" ht="13.5" customHeight="1" s="91">
       <c r="A7" s="45" t="n"/>
       <c r="B7" s="19" t="inlineStr">
         <is>
@@ -6993,7 +6993,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="13.5" r="8" s="91" thickBot="1">
+    <row r="8" ht="13.5" customHeight="1" s="91" thickBot="1">
       <c r="A8" s="50" t="n"/>
       <c r="B8" s="19" t="inlineStr">
         <is>
@@ -7042,7 +7042,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="13.5" r="9" s="91" thickTop="1">
+    <row r="9" ht="13.5" customHeight="1" s="91" thickTop="1">
       <c r="A9" s="1" t="inlineStr">
         <is>
           <t>Notes</t>
@@ -7089,7 +7089,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="13.5" r="10" s="91">
+    <row r="10" ht="13.5" customHeight="1" s="91">
       <c r="A10" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">   PCF = Probe Correction Factor</t>
@@ -7134,7 +7134,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="13.5" r="11" s="91">
+    <row r="11" ht="13.5" customHeight="1" s="91">
       <c r="A11" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">   Tb = Background count time</t>
@@ -7179,7 +7179,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="13.5" r="12" s="91">
+    <row r="12" ht="13.5" customHeight="1" s="91">
       <c r="A12" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">   Ts = Sample count time</t>
@@ -7221,7 +7221,7 @@
       <c r="S12" s="496" t="n"/>
       <c r="V12" s="30" t="n"/>
     </row>
-    <row customHeight="1" ht="13.5" r="13" s="91">
+    <row r="13" ht="13.5" customHeight="1" s="91">
       <c r="A13" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">   Rb = Background count rate</t>
@@ -7263,7 +7263,7 @@
       <c r="S13" s="496" t="n"/>
       <c r="V13" s="30" t="n"/>
     </row>
-    <row customHeight="1" ht="13.5" r="14" s="91">
+    <row r="14" ht="13.5" customHeight="1" s="91">
       <c r="A14" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">   Bcpm = Background cpm </t>
@@ -7300,7 +7300,7 @@
       <c r="S14" s="496" t="n"/>
       <c r="V14" s="30" t="n"/>
     </row>
-    <row customHeight="1" ht="13.5" r="15" s="91">
+    <row r="15" ht="13.5" customHeight="1" s="91">
       <c r="A15" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">   MDCR = Minimum Detectable Count Rate (net cpm)</t>
@@ -7341,7 +7341,7 @@
       <c r="S15" s="496" t="n"/>
       <c r="V15" s="30" t="n"/>
     </row>
-    <row customHeight="1" ht="13.5" r="16" s="91" thickBot="1">
+    <row r="16" ht="13.5" customHeight="1" s="91" thickBot="1">
       <c r="A16" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">   MDC = Minimum Detectable Concentration (dpm per 100cm2)</t>
@@ -7383,7 +7383,7 @@
       <c r="S16" s="512" t="n"/>
       <c r="V16" s="30" t="n"/>
     </row>
-    <row customHeight="1" ht="24" r="17" s="91" thickBot="1" thickTop="1">
+    <row r="17" ht="24" customHeight="1" s="91" thickBot="1" thickTop="1">
       <c r="A17" s="6" t="inlineStr">
         <is>
           <t>No.</t>
@@ -7456,7 +7456,7 @@
         </is>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.6" r="18" s="80" thickTop="1">
+    <row r="18" ht="15.6" customFormat="1" customHeight="1" s="80" thickTop="1">
       <c r="A18" s="98" t="n">
         <v>1</v>
       </c>
@@ -7499,7 +7499,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.6" r="19" s="80">
+    <row r="19" ht="15.6" customFormat="1" customHeight="1" s="80">
       <c r="A19" s="102" t="n">
         <v>2</v>
       </c>
@@ -7546,7 +7546,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.6" r="20" s="80">
+    <row r="20" ht="15.6" customFormat="1" customHeight="1" s="80">
       <c r="A20" s="98" t="n">
         <v>3</v>
       </c>
@@ -7593,7 +7593,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.6" r="21" s="80">
+    <row r="21" ht="15.6" customFormat="1" customHeight="1" s="80">
       <c r="A21" s="102" t="n">
         <v>4</v>
       </c>
@@ -7636,7 +7636,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.6" r="22" s="80">
+    <row r="22" ht="15.6" customFormat="1" customHeight="1" s="80">
       <c r="A22" s="98" t="n">
         <v>5</v>
       </c>
@@ -7683,7 +7683,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.6" r="23" s="80">
+    <row r="23" ht="15.6" customFormat="1" customHeight="1" s="80">
       <c r="A23" s="98" t="n">
         <v>6</v>
       </c>
@@ -7730,7 +7730,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.6" r="24" s="80">
+    <row r="24" ht="15.6" customFormat="1" customHeight="1" s="80">
       <c r="A24" s="102" t="n">
         <v>7</v>
       </c>
@@ -7773,7 +7773,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.6" r="25" s="80">
+    <row r="25" ht="15.6" customFormat="1" customHeight="1" s="80">
       <c r="A25" s="98" t="n">
         <v>8</v>
       </c>
@@ -7820,7 +7820,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.6" r="26" s="80">
+    <row r="26" ht="15.6" customFormat="1" customHeight="1" s="80">
       <c r="A26" s="98" t="n">
         <v>9</v>
       </c>
@@ -7867,7 +7867,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.6" r="27" s="80">
+    <row r="27" ht="15.6" customFormat="1" customHeight="1" s="80">
       <c r="A27" s="102" t="n"/>
       <c r="B27" s="599" t="n"/>
       <c r="C27" s="495" t="n"/>
@@ -7900,7 +7900,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.6" r="28" s="80">
+    <row r="28" ht="15.6" customFormat="1" customHeight="1" s="80">
       <c r="A28" s="98" t="n"/>
       <c r="B28" s="599" t="n"/>
       <c r="C28" s="495" t="n"/>
@@ -7933,7 +7933,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.6" r="29" s="80">
+    <row r="29" ht="15.6" customFormat="1" customHeight="1" s="80">
       <c r="A29" s="102" t="n"/>
       <c r="B29" s="599" t="n"/>
       <c r="C29" s="495" t="n"/>
@@ -7971,7 +7971,7 @@
         </is>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.6" r="30" s="80">
+    <row r="30" ht="15.6" customFormat="1" customHeight="1" s="80">
       <c r="A30" s="98" t="n"/>
       <c r="B30" s="599" t="n"/>
       <c r="C30" s="495" t="n"/>
@@ -8004,7 +8004,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.6" r="31" s="80">
+    <row r="31" ht="15.6" customFormat="1" customHeight="1" s="80">
       <c r="A31" s="102" t="n"/>
       <c r="B31" s="599" t="n"/>
       <c r="C31" s="495" t="n"/>
@@ -8037,7 +8037,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.6" r="32" s="80">
+    <row r="32" ht="15.6" customFormat="1" customHeight="1" s="80">
       <c r="A32" s="98" t="n"/>
       <c r="B32" s="599" t="n"/>
       <c r="C32" s="495" t="n"/>
@@ -8070,7 +8070,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.6" r="33" s="80">
+    <row r="33" ht="15.6" customFormat="1" customHeight="1" s="80">
       <c r="A33" s="102" t="n"/>
       <c r="B33" s="599" t="n"/>
       <c r="C33" s="495" t="n"/>
@@ -8103,7 +8103,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.6" r="34" s="80">
+    <row r="34" ht="15.6" customFormat="1" customHeight="1" s="80">
       <c r="A34" s="98" t="n"/>
       <c r="B34" s="599" t="n"/>
       <c r="C34" s="495" t="n"/>
@@ -8136,7 +8136,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.6" r="35" s="80">
+    <row r="35" ht="15.6" customFormat="1" customHeight="1" s="80">
       <c r="A35" s="102" t="n"/>
       <c r="B35" s="599" t="n"/>
       <c r="C35" s="495" t="n"/>
@@ -8169,7 +8169,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.6" r="36" s="80">
+    <row r="36" ht="15.6" customFormat="1" customHeight="1" s="80">
       <c r="A36" s="98" t="n"/>
       <c r="B36" s="599" t="n"/>
       <c r="C36" s="495" t="n"/>
@@ -8202,7 +8202,7 @@
         <v/>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.6" r="37" s="80" thickBot="1">
+    <row r="37" ht="15.6" customFormat="1" customHeight="1" s="80" thickBot="1">
       <c r="A37" s="106" t="n"/>
       <c r="B37" s="600" t="n"/>
       <c r="C37" s="511" t="n"/>
@@ -8235,7 +8235,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="38" s="91" thickTop="1">
+    <row r="38" ht="15.75" customHeight="1" s="91" thickTop="1">
       <c r="A38" s="84" t="n"/>
       <c r="B38" s="84" t="n"/>
       <c r="C38" s="85" t="n"/>
@@ -8295,7 +8295,7 @@
       <c r="BB38" s="90" t="n"/>
       <c r="BC38" s="90" t="n"/>
     </row>
-    <row customHeight="1" ht="15.75" r="39" s="91">
+    <row r="39" ht="15.75" customHeight="1" s="91">
       <c r="A39" s="395" t="n"/>
       <c r="O39" s="391" t="n"/>
       <c r="T39" s="90" t="n"/>
@@ -8446,8 +8446,8 @@
     <mergeCell ref="A39:N39"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
-  <pageMargins bottom="0.25" footer="0.1" header="0.375" left="0.25" right="0.25" top="0.25"/>
-  <pageSetup fitToHeight="0" orientation="landscape" scale="97"/>
+  <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.375" footer="0.1"/>
+  <pageSetup orientation="landscape" scale="97" fitToHeight="0"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"_x000a_                                                            </oddHeader>
     <oddFooter/>
@@ -8467,16 +8467,16 @@
   </sheetPr>
   <dimension ref="A1:DH56"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AK42" sqref="AK42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="1.7109375" defaultRowHeight="12"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="1.7109375" defaultRowHeight="12" customHeight="1"/>
   <cols>
-    <col customWidth="1" max="16384" min="1" style="153" width="1.7109375"/>
+    <col width="1.7109375" customWidth="1" style="153" min="1" max="16384"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="38.25" r="1" s="91" thickBot="1">
+    <row r="1" ht="38.25" customHeight="1" s="91" thickBot="1">
       <c r="A1" s="479" t="n"/>
       <c r="B1" s="506" t="n"/>
       <c r="C1" s="506" t="n"/>
@@ -8555,7 +8555,7 @@
       <c r="BX1" s="506" t="n"/>
       <c r="BY1" s="506" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="2" s="91" thickTop="1">
+    <row r="2" ht="12" customHeight="1" s="91" thickTop="1">
       <c r="A2" s="118" t="n"/>
       <c r="B2" s="119" t="n"/>
       <c r="C2" s="119" t="n"/>
@@ -8634,7 +8634,7 @@
       <c r="BX2" s="119" t="n"/>
       <c r="BY2" s="120" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="3" s="91">
+    <row r="3" ht="12" customHeight="1" s="91">
       <c r="A3" s="121" t="n"/>
       <c r="B3" s="122" t="n"/>
       <c r="C3" s="123" t="n"/>
@@ -8713,7 +8713,7 @@
       <c r="BX3" s="123" t="n"/>
       <c r="BY3" s="124" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="4" s="91">
+    <row r="4" ht="12" customHeight="1" s="91">
       <c r="A4" s="121" t="n"/>
       <c r="B4" s="123" t="n"/>
       <c r="C4" s="123" t="n"/>
@@ -8792,7 +8792,7 @@
       <c r="BX4" s="123" t="n"/>
       <c r="BY4" s="124" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="5" s="91">
+    <row r="5" ht="12" customHeight="1" s="91">
       <c r="A5" s="136" t="n"/>
       <c r="B5" s="153" t="n"/>
       <c r="C5" s="153" t="n"/>
@@ -8871,7 +8871,7 @@
       <c r="BX5" s="153" t="n"/>
       <c r="BY5" s="128" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="6" s="91">
+    <row r="6" ht="12" customHeight="1" s="91">
       <c r="A6" s="136" t="n"/>
       <c r="B6" s="153" t="n"/>
       <c r="C6" s="153" t="n"/>
@@ -8950,7 +8950,7 @@
       <c r="BX6" s="153" t="n"/>
       <c r="BY6" s="128" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="7" s="91">
+    <row r="7" ht="12" customHeight="1" s="91">
       <c r="A7" s="136" t="n"/>
       <c r="B7" s="153" t="n"/>
       <c r="C7" s="153" t="n"/>
@@ -9029,7 +9029,7 @@
       <c r="BX7" s="153" t="n"/>
       <c r="BY7" s="128" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="8" s="91">
+    <row r="8" ht="12" customHeight="1" s="91">
       <c r="A8" s="136" t="n"/>
       <c r="B8" s="153" t="n"/>
       <c r="C8" s="153" t="n"/>
@@ -9108,7 +9108,7 @@
       <c r="BX8" s="153" t="n"/>
       <c r="BY8" s="128" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="9" s="91">
+    <row r="9" ht="12" customHeight="1" s="91">
       <c r="A9" s="136" t="n"/>
       <c r="B9" s="153" t="n"/>
       <c r="C9" s="153" t="n"/>
@@ -9187,7 +9187,7 @@
       <c r="BX9" s="153" t="n"/>
       <c r="BY9" s="128" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="10" s="91">
+    <row r="10" ht="12" customHeight="1" s="91">
       <c r="A10" s="136" t="n"/>
       <c r="B10" s="153" t="n"/>
       <c r="C10" s="153" t="n"/>
@@ -9266,7 +9266,7 @@
       <c r="BX10" s="153" t="n"/>
       <c r="BY10" s="128" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="11" s="91">
+    <row r="11" ht="12" customHeight="1" s="91">
       <c r="A11" s="136" t="n"/>
       <c r="B11" s="153" t="n"/>
       <c r="C11" s="153" t="n"/>
@@ -9345,7 +9345,7 @@
       <c r="BX11" s="153" t="n"/>
       <c r="BY11" s="128" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="12" s="91">
+    <row r="12" ht="12" customHeight="1" s="91">
       <c r="A12" s="136" t="n"/>
       <c r="B12" s="153" t="n"/>
       <c r="C12" s="153" t="n"/>
@@ -9424,7 +9424,7 @@
       <c r="BX12" s="153" t="n"/>
       <c r="BY12" s="128" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="13" s="91">
+    <row r="13" ht="12" customHeight="1" s="91">
       <c r="A13" s="136" t="n"/>
       <c r="B13" s="153" t="n"/>
       <c r="C13" s="153" t="n"/>
@@ -9503,7 +9503,7 @@
       <c r="BX13" s="153" t="n"/>
       <c r="BY13" s="128" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="14" s="91">
+    <row r="14" ht="12" customHeight="1" s="91">
       <c r="A14" s="136" t="n"/>
       <c r="B14" s="153" t="n"/>
       <c r="C14" s="153" t="n"/>
@@ -9582,7 +9582,7 @@
       <c r="BX14" s="153" t="n"/>
       <c r="BY14" s="128" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="15" s="91">
+    <row r="15" ht="12" customHeight="1" s="91">
       <c r="A15" s="136" t="n"/>
       <c r="B15" s="153" t="n"/>
       <c r="C15" s="153" t="n"/>
@@ -9680,7 +9680,7 @@
       <c r="DG15" s="160" t="n"/>
       <c r="DH15" s="160" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="16" s="91">
+    <row r="16" ht="12" customHeight="1" s="91">
       <c r="A16" s="136" t="n"/>
       <c r="B16" s="153" t="n"/>
       <c r="C16" s="153" t="n"/>
@@ -9778,7 +9778,7 @@
       <c r="DG16" s="160" t="n"/>
       <c r="DH16" s="160" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="17" s="91">
+    <row r="17" ht="12" customHeight="1" s="91">
       <c r="A17" s="136" t="n"/>
       <c r="B17" s="153" t="n"/>
       <c r="C17" s="153" t="n"/>
@@ -9876,7 +9876,7 @@
       <c r="DG17" s="160" t="n"/>
       <c r="DH17" s="160" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="18" s="91">
+    <row r="18" ht="12" customHeight="1" s="91">
       <c r="A18" s="136" t="n"/>
       <c r="B18" s="153" t="n"/>
       <c r="C18" s="153" t="n"/>
@@ -9974,7 +9974,7 @@
       <c r="DG18" s="160" t="n"/>
       <c r="DH18" s="160" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="19" s="91">
+    <row r="19" ht="12" customHeight="1" s="91">
       <c r="A19" s="136" t="n"/>
       <c r="B19" s="153" t="n"/>
       <c r="C19" s="153" t="n"/>
@@ -10072,7 +10072,7 @@
       <c r="DG19" s="160" t="n"/>
       <c r="DH19" s="160" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="20" s="91">
+    <row r="20" ht="12" customHeight="1" s="91">
       <c r="A20" s="136" t="n"/>
       <c r="B20" s="153" t="n"/>
       <c r="C20" s="153" t="n"/>
@@ -10170,7 +10170,7 @@
       <c r="DG20" s="160" t="n"/>
       <c r="DH20" s="160" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="21" s="91">
+    <row r="21" ht="12" customHeight="1" s="91">
       <c r="A21" s="136" t="n"/>
       <c r="B21" s="153" t="n"/>
       <c r="C21" s="153" t="n"/>
@@ -10268,7 +10268,7 @@
       <c r="DG21" s="160" t="n"/>
       <c r="DH21" s="160" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="22" s="91">
+    <row r="22" ht="12" customHeight="1" s="91">
       <c r="A22" s="136" t="n"/>
       <c r="B22" s="153" t="n"/>
       <c r="C22" s="153" t="n"/>
@@ -10366,7 +10366,7 @@
       <c r="DG22" s="160" t="n"/>
       <c r="DH22" s="160" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="23" s="91">
+    <row r="23" ht="12" customHeight="1" s="91">
       <c r="A23" s="136" t="n"/>
       <c r="B23" s="153" t="n"/>
       <c r="C23" s="153" t="n"/>
@@ -10464,7 +10464,7 @@
       <c r="DG23" s="160" t="n"/>
       <c r="DH23" s="160" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="24" s="91">
+    <row r="24" ht="12" customHeight="1" s="91">
       <c r="A24" s="136" t="n"/>
       <c r="B24" s="153" t="n"/>
       <c r="C24" s="153" t="n"/>
@@ -10543,7 +10543,7 @@
       <c r="BX24" s="153" t="n"/>
       <c r="BY24" s="128" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="25" s="91">
+    <row r="25" ht="12" customHeight="1" s="91">
       <c r="A25" s="136" t="n"/>
       <c r="B25" s="153" t="n"/>
       <c r="C25" s="153" t="n"/>
@@ -10622,7 +10622,7 @@
       <c r="BX25" s="153" t="n"/>
       <c r="BY25" s="128" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="26" s="91">
+    <row r="26" ht="12" customHeight="1" s="91">
       <c r="A26" s="136" t="n"/>
       <c r="B26" s="153" t="n"/>
       <c r="C26" s="153" t="n"/>
@@ -10701,7 +10701,7 @@
       <c r="BX26" s="153" t="n"/>
       <c r="BY26" s="128" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="27" s="91">
+    <row r="27" ht="12" customHeight="1" s="91">
       <c r="A27" s="136" t="n"/>
       <c r="B27" s="160" t="n"/>
       <c r="C27" s="160" t="n"/>
@@ -10780,7 +10780,7 @@
       <c r="BX27" s="153" t="n"/>
       <c r="BY27" s="128" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="28" s="91">
+    <row r="28" ht="12" customHeight="1" s="91">
       <c r="A28" s="136" t="n"/>
       <c r="B28" s="160" t="n"/>
       <c r="C28" s="160" t="n"/>
@@ -10859,7 +10859,7 @@
       <c r="BX28" s="153" t="n"/>
       <c r="BY28" s="128" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="29" s="91">
+    <row r="29" ht="12" customHeight="1" s="91">
       <c r="A29" s="136" t="n"/>
       <c r="B29" s="160" t="n"/>
       <c r="C29" s="160" t="n"/>
@@ -10938,7 +10938,7 @@
       <c r="BX29" s="153" t="n"/>
       <c r="BY29" s="128" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="30" s="91">
+    <row r="30" ht="12" customHeight="1" s="91">
       <c r="A30" s="136" t="n"/>
       <c r="B30" s="160" t="n"/>
       <c r="C30" s="160" t="n"/>
@@ -11017,7 +11017,7 @@
       <c r="BX30" s="153" t="n"/>
       <c r="BY30" s="128" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="31" s="91">
+    <row r="31" ht="12" customHeight="1" s="91">
       <c r="A31" s="136" t="n"/>
       <c r="B31" s="160" t="n"/>
       <c r="C31" s="160" t="n"/>
@@ -11096,7 +11096,7 @@
       <c r="BX31" s="153" t="n"/>
       <c r="BY31" s="128" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="32" s="91">
+    <row r="32" ht="12" customHeight="1" s="91">
       <c r="A32" s="136" t="n"/>
       <c r="B32" s="160" t="n"/>
       <c r="C32" s="160" t="n"/>
@@ -11175,7 +11175,7 @@
       <c r="BX32" s="153" t="n"/>
       <c r="BY32" s="128" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="33" s="91">
+    <row r="33" ht="12" customHeight="1" s="91">
       <c r="A33" s="136" t="n"/>
       <c r="B33" s="160" t="n"/>
       <c r="C33" s="160" t="n"/>
@@ -11254,7 +11254,7 @@
       <c r="BX33" s="153" t="n"/>
       <c r="BY33" s="128" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="34" s="91">
+    <row r="34" ht="12" customHeight="1" s="91">
       <c r="A34" s="136" t="n"/>
       <c r="B34" s="160" t="n"/>
       <c r="C34" s="160" t="n"/>
@@ -11333,7 +11333,7 @@
       <c r="BX34" s="153" t="n"/>
       <c r="BY34" s="128" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="35" s="91">
+    <row r="35" ht="12" customHeight="1" s="91">
       <c r="A35" s="136" t="n"/>
       <c r="B35" s="160" t="n"/>
       <c r="C35" s="160" t="n"/>
@@ -11412,7 +11412,7 @@
       <c r="BX35" s="153" t="n"/>
       <c r="BY35" s="128" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="36" s="91">
+    <row r="36" ht="12" customHeight="1" s="91">
       <c r="A36" s="136" t="n"/>
       <c r="B36" s="160" t="n"/>
       <c r="C36" s="160" t="n"/>
@@ -11491,7 +11491,7 @@
       <c r="BX36" s="153" t="n"/>
       <c r="BY36" s="128" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="37" s="91" thickBot="1">
+    <row r="37" ht="12" customHeight="1" s="91" thickBot="1">
       <c r="A37" s="141" t="n"/>
       <c r="B37" s="144" t="n"/>
       <c r="C37" s="144" t="n"/>
@@ -11570,7 +11570,7 @@
       <c r="BX37" s="144" t="n"/>
       <c r="BY37" s="145" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="38" s="91" thickTop="1">
+    <row r="38" ht="12" customHeight="1" s="91" thickTop="1">
       <c r="A38" s="499" t="inlineStr">
         <is>
           <t>Survey No</t>
@@ -11657,7 +11657,7 @@
       <c r="BX38" s="146" t="n"/>
       <c r="BY38" s="149" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="39" s="91">
+    <row r="39" ht="12" customHeight="1" s="91">
       <c r="A39" s="528" t="inlineStr">
         <is>
           <t>Date</t>
@@ -11742,7 +11742,7 @@
       <c r="BX39" s="213" t="n"/>
       <c r="BY39" s="151" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="40" s="91">
+    <row r="40" ht="12" customHeight="1" s="91">
       <c r="A40" s="528" t="inlineStr">
         <is>
           <t>Survey Tech</t>
@@ -11852,7 +11852,7 @@
       <c r="CU40" s="153" t="n"/>
       <c r="CV40" s="153" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="41" s="91">
+    <row r="41" ht="12" customHeight="1" s="91">
       <c r="A41" s="528" t="inlineStr">
         <is>
           <t>Count Room Tech</t>
@@ -11962,7 +11962,7 @@
       <c r="CU41" s="153" t="n"/>
       <c r="CV41" s="153" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="42" s="91">
+    <row r="42" ht="12" customHeight="1" s="91">
       <c r="A42" s="528" t="inlineStr">
         <is>
           <t>Date Counted</t>
@@ -12070,7 +12070,7 @@
       <c r="CU42" s="153" t="n"/>
       <c r="CV42" s="153" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="43" s="91">
+    <row r="43" ht="12" customHeight="1" s="91">
       <c r="A43" s="528" t="inlineStr">
         <is>
           <t>Survey Type</t>
@@ -12180,7 +12180,7 @@
       <c r="CU43" s="153" t="n"/>
       <c r="CV43" s="153" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="44" s="91">
+    <row r="44" ht="12" customHeight="1" s="91">
       <c r="A44" s="528" t="inlineStr">
         <is>
           <t>Level of Posting</t>
@@ -12290,7 +12290,7 @@
       <c r="CU44" s="153" t="n"/>
       <c r="CV44" s="153" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="45" s="91" thickBot="1">
+    <row r="45" ht="12" customHeight="1" s="91" thickBot="1">
       <c r="A45" s="604" t="inlineStr">
         <is>
           <t>Comments</t>
@@ -12396,10 +12396,10 @@
       <c r="CU45" s="153" t="n"/>
       <c r="CV45" s="153" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="46" s="91" thickTop="1"/>
+    <row r="46" ht="12" customHeight="1" s="91" thickTop="1"/>
     <row r="47"/>
     <row r="48"/>
-    <row customHeight="1" ht="12" r="49" s="91">
+    <row r="49" ht="12" customHeight="1" s="91">
       <c r="A49" s="153" t="n"/>
       <c r="B49" s="153" t="n"/>
       <c r="C49" s="153" t="n"/>
@@ -12407,7 +12407,7 @@
       <c r="E49" s="153" t="n"/>
       <c r="F49" s="153" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="50" s="91">
+    <row r="50" ht="12" customHeight="1" s="91">
       <c r="A50" s="153" t="n"/>
       <c r="B50" s="153" t="n"/>
       <c r="C50" s="153" t="n"/>
@@ -12415,7 +12415,7 @@
       <c r="E50" s="153" t="n"/>
       <c r="F50" s="153" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="51" s="91">
+    <row r="51" ht="12" customHeight="1" s="91">
       <c r="A51" s="160" t="n"/>
       <c r="B51" s="160" t="n"/>
       <c r="C51" s="153" t="n"/>
@@ -12423,7 +12423,7 @@
       <c r="E51" s="153" t="n"/>
       <c r="F51" s="153" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="52" s="91">
+    <row r="52" ht="12" customHeight="1" s="91">
       <c r="A52" s="160" t="n"/>
       <c r="B52" s="160" t="n"/>
       <c r="C52" s="153" t="n"/>
@@ -12431,7 +12431,7 @@
       <c r="E52" s="153" t="n"/>
       <c r="F52" s="153" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="53" s="91">
+    <row r="53" ht="12" customHeight="1" s="91">
       <c r="A53" s="153" t="n"/>
       <c r="B53" s="153" t="n"/>
       <c r="C53" s="153" t="n"/>
@@ -12439,7 +12439,7 @@
       <c r="E53" s="153" t="n"/>
       <c r="F53" s="153" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="54" s="91">
+    <row r="54" ht="12" customHeight="1" s="91">
       <c r="A54" s="153" t="n"/>
       <c r="B54" s="153" t="n"/>
       <c r="C54" s="153" t="n"/>
@@ -12447,7 +12447,7 @@
       <c r="E54" s="153" t="n"/>
       <c r="F54" s="153" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="55" s="91">
+    <row r="55" ht="12" customHeight="1" s="91">
       <c r="A55" s="153" t="n"/>
       <c r="B55" s="153" t="n"/>
       <c r="C55" s="153" t="n"/>
@@ -12455,7 +12455,7 @@
       <c r="E55" s="153" t="n"/>
       <c r="F55" s="153" t="n"/>
     </row>
-    <row customHeight="1" ht="12" r="56" s="91">
+    <row r="56" ht="12" customHeight="1" s="91">
       <c r="A56" s="153" t="n"/>
       <c r="B56" s="153" t="n"/>
       <c r="C56" s="153" t="n"/>
@@ -12484,8 +12484,8 @@
     <mergeCell ref="K39:Y39"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
-  <pageMargins bottom="0.25" footer="0.1" header="0.375" left="0.25" right="0.25" top="0.25"/>
-  <pageSetup fitToHeight="0" orientation="landscape"/>
+  <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.375" footer="0.1"/>
+  <pageSetup orientation="landscape" fitToHeight="0"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"_x000a_                                                            </oddHeader>
     <oddFooter/>

</xml_diff>